<commit_message>
Restructured how data is implemented for app
</commit_message>
<xml_diff>
--- a/test/dummy_data/test_data1.xlsx
+++ b/test/dummy_data/test_data1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D'Andre House\Codes\Budget_app\test\dummy_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D79DC5-415F-41C3-B78A-785AE6186D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5088160F-8224-4868-A989-C1BF9994270B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D8CC8EF-BED7-4D81-99B7-B5B4BB8EE65A}"/>
   </bookViews>
@@ -313,7 +313,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -346,7 +346,7 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -742,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4543D05F-42C8-4C63-9942-416653535C02}">
-  <dimension ref="A1:I218"/>
+  <dimension ref="A1:K218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="C216" sqref="C216"/>
+    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
+      <selection activeCell="M205" sqref="M205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +760,7 @@
     <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>44928</v>
       </c>
@@ -788,8 +788,14 @@
       <c r="I1" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="4">
+        <v>4</v>
+      </c>
+      <c r="K1" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44929</v>
       </c>
@@ -817,8 +823,14 @@
       <c r="I2" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="4">
+        <v>8</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44931</v>
       </c>
@@ -846,8 +858,14 @@
       <c r="I3" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="4">
+        <v>8</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44931</v>
       </c>
@@ -875,8 +893,14 @@
       <c r="I4" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="4">
+        <v>8</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44934</v>
       </c>
@@ -904,8 +928,14 @@
       <c r="I5" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="4">
+        <v>8</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44956</v>
       </c>
@@ -933,8 +963,14 @@
       <c r="I6" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="4">
+        <v>8</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44932</v>
       </c>
@@ -962,8 +998,14 @@
       <c r="I7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="4">
+        <v>8</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44932</v>
       </c>
@@ -991,8 +1033,14 @@
       <c r="I8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="4">
+        <v>8</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44936</v>
       </c>
@@ -1020,8 +1068,14 @@
       <c r="I9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="4">
+        <v>8</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44937</v>
       </c>
@@ -1049,8 +1103,14 @@
       <c r="I10" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="4">
+        <v>4</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44937</v>
       </c>
@@ -1078,8 +1138,14 @@
       <c r="I11" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="4">
+        <v>8</v>
+      </c>
+      <c r="K11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44938</v>
       </c>
@@ -1107,8 +1173,14 @@
       <c r="I12" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="4">
+        <v>4</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44940</v>
       </c>
@@ -1136,8 +1208,14 @@
       <c r="I13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="4">
+        <v>8</v>
+      </c>
+      <c r="K13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44942</v>
       </c>
@@ -1165,8 +1243,14 @@
       <c r="I14" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="4">
+        <v>8</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44942</v>
       </c>
@@ -1194,8 +1278,14 @@
       <c r="I15" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="4">
+        <v>8</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44945</v>
       </c>
@@ -1223,8 +1313,14 @@
       <c r="I16" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="4">
+        <v>8</v>
+      </c>
+      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44945</v>
       </c>
@@ -1252,8 +1348,14 @@
       <c r="I17" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="4">
+        <v>8</v>
+      </c>
+      <c r="K17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44946</v>
       </c>
@@ -1281,8 +1383,14 @@
       <c r="I18" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="4">
+        <v>4</v>
+      </c>
+      <c r="K18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44945</v>
       </c>
@@ -1310,8 +1418,14 @@
       <c r="I19" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="4">
+        <v>8</v>
+      </c>
+      <c r="K19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44948</v>
       </c>
@@ -1339,8 +1453,14 @@
       <c r="I20" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="4">
+        <v>8</v>
+      </c>
+      <c r="K20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44948</v>
       </c>
@@ -1368,8 +1488,14 @@
       <c r="I21" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="4">
+        <v>8</v>
+      </c>
+      <c r="K21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44950</v>
       </c>
@@ -1397,8 +1523,14 @@
       <c r="I22" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="4">
+        <v>8</v>
+      </c>
+      <c r="K22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44951</v>
       </c>
@@ -1426,8 +1558,14 @@
       <c r="I23" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="4">
+        <v>8</v>
+      </c>
+      <c r="K23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44952</v>
       </c>
@@ -1455,8 +1593,14 @@
       <c r="I24" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="4">
+        <v>8</v>
+      </c>
+      <c r="K24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44954</v>
       </c>
@@ -1484,8 +1628,14 @@
       <c r="I25" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="4">
+        <v>8</v>
+      </c>
+      <c r="K25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44954</v>
       </c>
@@ -1513,8 +1663,14 @@
       <c r="I26" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="4">
+        <v>8</v>
+      </c>
+      <c r="K26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44954</v>
       </c>
@@ -1542,8 +1698,14 @@
       <c r="I27" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="4">
+        <v>8</v>
+      </c>
+      <c r="K27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44956</v>
       </c>
@@ -1571,8 +1733,14 @@
       <c r="I28" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="4">
+        <v>8</v>
+      </c>
+      <c r="K28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44932</v>
       </c>
@@ -1600,8 +1768,14 @@
       <c r="I29" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="4">
+        <v>8</v>
+      </c>
+      <c r="K29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44935</v>
       </c>
@@ -1629,8 +1803,14 @@
       <c r="I30" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="4">
+        <v>8</v>
+      </c>
+      <c r="K30" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44946</v>
       </c>
@@ -1658,8 +1838,14 @@
       <c r="I31" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="4">
+        <v>8</v>
+      </c>
+      <c r="K31" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44950</v>
       </c>
@@ -1687,8 +1873,14 @@
       <c r="I32" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="4">
+        <v>8</v>
+      </c>
+      <c r="K32" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44930</v>
       </c>
@@ -1716,8 +1908,14 @@
       <c r="I33" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="4">
+        <v>4</v>
+      </c>
+      <c r="K33" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44930</v>
       </c>
@@ -1745,8 +1943,14 @@
       <c r="I34" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="4">
+        <v>8</v>
+      </c>
+      <c r="K34" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44930</v>
       </c>
@@ -1774,8 +1978,14 @@
       <c r="I35" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="4">
+        <v>4</v>
+      </c>
+      <c r="K35" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44938</v>
       </c>
@@ -1803,8 +2013,14 @@
       <c r="I36" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="4">
+        <v>4</v>
+      </c>
+      <c r="K36" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44946</v>
       </c>
@@ -1832,8 +2048,14 @@
       <c r="I37" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="4">
+        <v>4</v>
+      </c>
+      <c r="K37" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44949</v>
       </c>
@@ -1861,8 +2083,14 @@
       <c r="I38" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="4">
+        <v>8</v>
+      </c>
+      <c r="K38" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44949</v>
       </c>
@@ -1890,8 +2118,14 @@
       <c r="I39" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="4">
+        <v>8</v>
+      </c>
+      <c r="K39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44951</v>
       </c>
@@ -1919,8 +2153,14 @@
       <c r="I40" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="4">
+        <v>4</v>
+      </c>
+      <c r="K40" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44929</v>
       </c>
@@ -1948,8 +2188,14 @@
       <c r="I41" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="4">
+        <v>8</v>
+      </c>
+      <c r="K41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44931</v>
       </c>
@@ -1977,8 +2223,14 @@
       <c r="I42" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="4">
+        <v>8</v>
+      </c>
+      <c r="K42" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44939</v>
       </c>
@@ -2006,8 +2258,14 @@
       <c r="I43" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="4">
+        <v>8</v>
+      </c>
+      <c r="K43" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44956</v>
       </c>
@@ -2035,8 +2293,14 @@
       <c r="I44" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="4">
+        <v>8</v>
+      </c>
+      <c r="K44" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44942</v>
       </c>
@@ -2064,8 +2328,14 @@
       <c r="I45" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="4">
+        <v>8</v>
+      </c>
+      <c r="K45" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44946</v>
       </c>
@@ -2093,8 +2363,14 @@
       <c r="I46" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="4">
+        <v>8</v>
+      </c>
+      <c r="K46" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44947</v>
       </c>
@@ -2122,8 +2398,14 @@
       <c r="I47" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="4">
+        <v>8</v>
+      </c>
+      <c r="K47" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44947</v>
       </c>
@@ -2151,8 +2433,14 @@
       <c r="I48" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="4">
+        <v>8</v>
+      </c>
+      <c r="K48" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44950</v>
       </c>
@@ -2180,8 +2468,14 @@
       <c r="I49" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="4">
+        <v>8</v>
+      </c>
+      <c r="K49" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44956</v>
       </c>
@@ -2209,8 +2503,14 @@
       <c r="I50" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" s="4">
+        <v>8</v>
+      </c>
+      <c r="K50" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44956</v>
       </c>
@@ -2238,8 +2538,14 @@
       <c r="I51" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="4">
+        <v>8</v>
+      </c>
+      <c r="K51" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44950</v>
       </c>
@@ -2267,8 +2573,14 @@
       <c r="I52" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="4">
+        <v>8</v>
+      </c>
+      <c r="K52" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44950</v>
       </c>
@@ -2296,8 +2608,14 @@
       <c r="I53" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" s="4">
+        <v>8</v>
+      </c>
+      <c r="K53" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44956</v>
       </c>
@@ -2325,8 +2643,14 @@
       <c r="I54" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" s="4">
+        <v>8</v>
+      </c>
+      <c r="K54" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44957</v>
       </c>
@@ -2354,8 +2678,14 @@
       <c r="I55" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" s="4">
+        <v>4</v>
+      </c>
+      <c r="K55" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44956</v>
       </c>
@@ -2383,8 +2713,14 @@
       <c r="I56" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" s="4">
+        <v>8</v>
+      </c>
+      <c r="K56" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44957</v>
       </c>
@@ -2412,8 +2748,14 @@
       <c r="I57" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" s="4">
+        <v>4</v>
+      </c>
+      <c r="K57" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44960</v>
       </c>
@@ -2441,8 +2783,14 @@
       <c r="I58" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" s="4">
+        <v>8</v>
+      </c>
+      <c r="K58" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44971</v>
       </c>
@@ -2470,8 +2818,14 @@
       <c r="I59" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" s="4">
+        <v>8</v>
+      </c>
+      <c r="K59" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44970</v>
       </c>
@@ -2499,8 +2853,14 @@
       <c r="I60" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" s="4">
+        <v>8</v>
+      </c>
+      <c r="K60" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44958</v>
       </c>
@@ -2528,8 +2888,14 @@
       <c r="I61" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" s="4">
+        <v>4</v>
+      </c>
+      <c r="K61" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44958</v>
       </c>
@@ -2557,8 +2923,14 @@
       <c r="I62" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" s="4">
+        <v>4</v>
+      </c>
+      <c r="K62" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44963</v>
       </c>
@@ -2586,8 +2958,14 @@
       <c r="I63" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" s="4">
+        <v>4</v>
+      </c>
+      <c r="K63" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44970</v>
       </c>
@@ -2615,8 +2993,14 @@
       <c r="I64" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" s="4">
+        <v>4</v>
+      </c>
+      <c r="K64" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44978</v>
       </c>
@@ -2644,8 +3028,14 @@
       <c r="I65" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65" s="4">
+        <v>4</v>
+      </c>
+      <c r="K65" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44958</v>
       </c>
@@ -2673,8 +3063,14 @@
       <c r="I66" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66" s="4">
+        <v>4</v>
+      </c>
+      <c r="K66" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44958</v>
       </c>
@@ -2702,8 +3098,14 @@
       <c r="I67" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J67" s="4">
+        <v>8</v>
+      </c>
+      <c r="K67" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44959</v>
       </c>
@@ -2731,8 +3133,14 @@
       <c r="I68" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68" s="4">
+        <v>8</v>
+      </c>
+      <c r="K68" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44970</v>
       </c>
@@ -2760,8 +3168,14 @@
       <c r="I69" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" s="4">
+        <v>8</v>
+      </c>
+      <c r="K69" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44974</v>
       </c>
@@ -2789,8 +3203,14 @@
       <c r="I70" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J70" s="4">
+        <v>8</v>
+      </c>
+      <c r="K70" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44980</v>
       </c>
@@ -2818,8 +3238,14 @@
       <c r="I71" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J71" s="4">
+        <v>8</v>
+      </c>
+      <c r="K71" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44980</v>
       </c>
@@ -2847,8 +3273,14 @@
       <c r="I72" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J72" s="4">
+        <v>8</v>
+      </c>
+      <c r="K72" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44982</v>
       </c>
@@ -2876,8 +3308,14 @@
       <c r="I73" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J73" s="4">
+        <v>8</v>
+      </c>
+      <c r="K73" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44983</v>
       </c>
@@ -2905,8 +3343,14 @@
       <c r="I74" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J74" s="4">
+        <v>8</v>
+      </c>
+      <c r="K74" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44985</v>
       </c>
@@ -2934,8 +3378,14 @@
       <c r="I75" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J75" s="4">
+        <v>4</v>
+      </c>
+      <c r="K75" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44985</v>
       </c>
@@ -2963,8 +3413,14 @@
       <c r="I76" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J76" s="4">
+        <v>4</v>
+      </c>
+      <c r="K76" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44985</v>
       </c>
@@ -2992,8 +3448,14 @@
       <c r="I77" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J77" s="4">
+        <v>4</v>
+      </c>
+      <c r="K77" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44985</v>
       </c>
@@ -3021,8 +3483,14 @@
       <c r="I78" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J78" s="4">
+        <v>4</v>
+      </c>
+      <c r="K78" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44964</v>
       </c>
@@ -3050,8 +3518,14 @@
       <c r="I79" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J79" s="4">
+        <v>8</v>
+      </c>
+      <c r="K79" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44965</v>
       </c>
@@ -3079,8 +3553,14 @@
       <c r="I80" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80" s="4">
+        <v>8</v>
+      </c>
+      <c r="K80" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44967</v>
       </c>
@@ -3108,8 +3588,14 @@
       <c r="I81" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J81" s="4">
+        <v>8</v>
+      </c>
+      <c r="K81" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44968</v>
       </c>
@@ -3137,8 +3623,14 @@
       <c r="I82" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J82" s="4">
+        <v>8</v>
+      </c>
+      <c r="K82" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44967</v>
       </c>
@@ -3166,8 +3658,14 @@
       <c r="I83" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J83" s="4">
+        <v>8</v>
+      </c>
+      <c r="K83" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44969</v>
       </c>
@@ -3195,8 +3693,14 @@
       <c r="I84" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J84" s="4">
+        <v>8</v>
+      </c>
+      <c r="K84" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44974</v>
       </c>
@@ -3224,8 +3728,14 @@
       <c r="I85" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J85" s="4">
+        <v>4</v>
+      </c>
+      <c r="K85" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44974</v>
       </c>
@@ -3253,8 +3763,14 @@
       <c r="I86" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86" s="4">
+        <v>8</v>
+      </c>
+      <c r="K86" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44977</v>
       </c>
@@ -3282,8 +3798,14 @@
       <c r="I87" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J87" s="4">
+        <v>4</v>
+      </c>
+      <c r="K87" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44983</v>
       </c>
@@ -3311,8 +3833,14 @@
       <c r="I88" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J88" s="4">
+        <v>8</v>
+      </c>
+      <c r="K88" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44983</v>
       </c>
@@ -3340,8 +3868,14 @@
       <c r="I89" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J89" s="4">
+        <v>8</v>
+      </c>
+      <c r="K89" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44983</v>
       </c>
@@ -3369,8 +3903,14 @@
       <c r="I90" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J90" s="4">
+        <v>8</v>
+      </c>
+      <c r="K90" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44985</v>
       </c>
@@ -3398,8 +3938,14 @@
       <c r="I91" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J91" s="4">
+        <v>8</v>
+      </c>
+      <c r="K91" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44986</v>
       </c>
@@ -3427,8 +3973,14 @@
       <c r="I92" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J92" s="4">
+        <v>4</v>
+      </c>
+      <c r="K92" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44986</v>
       </c>
@@ -3456,8 +4008,14 @@
       <c r="I93" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J93" s="4">
+        <v>8</v>
+      </c>
+      <c r="K93" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44986</v>
       </c>
@@ -3485,8 +4043,14 @@
       <c r="I94" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J94" s="4">
+        <v>4</v>
+      </c>
+      <c r="K94" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44991</v>
       </c>
@@ -3514,8 +4078,14 @@
       <c r="I95" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J95" s="4">
+        <v>4</v>
+      </c>
+      <c r="K95" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44991</v>
       </c>
@@ -3543,8 +4113,14 @@
       <c r="I96" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J96" s="4">
+        <v>8</v>
+      </c>
+      <c r="K96" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44998</v>
       </c>
@@ -3572,8 +4148,14 @@
       <c r="I97" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J97" s="4">
+        <v>4</v>
+      </c>
+      <c r="K97" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>45005</v>
       </c>
@@ -3601,8 +4183,14 @@
       <c r="I98" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J98" s="4">
+        <v>8</v>
+      </c>
+      <c r="K98" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>45005</v>
       </c>
@@ -3630,8 +4218,14 @@
       <c r="I99" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J99" s="4">
+        <v>4</v>
+      </c>
+      <c r="K99" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>45012</v>
       </c>
@@ -3659,8 +4253,14 @@
       <c r="I100" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J100" s="4">
+        <v>8</v>
+      </c>
+      <c r="K100" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44994</v>
       </c>
@@ -3688,8 +4288,14 @@
       <c r="I101" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J101" s="4">
+        <v>8</v>
+      </c>
+      <c r="K101" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>45013</v>
       </c>
@@ -3717,8 +4323,14 @@
       <c r="I102" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J102" s="4">
+        <v>4</v>
+      </c>
+      <c r="K102" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>45016</v>
       </c>
@@ -3746,8 +4358,14 @@
       <c r="I103" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J103" s="4">
+        <v>4</v>
+      </c>
+      <c r="K103" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>45016</v>
       </c>
@@ -3775,8 +4393,14 @@
       <c r="I104" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J104" s="4">
+        <v>4</v>
+      </c>
+      <c r="K104" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>45016</v>
       </c>
@@ -3804,8 +4428,14 @@
       <c r="I105" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J105" s="4">
+        <v>4</v>
+      </c>
+      <c r="K105" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44988</v>
       </c>
@@ -3833,8 +4463,14 @@
       <c r="I106" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J106" s="4">
+        <v>8</v>
+      </c>
+      <c r="K106" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44995</v>
       </c>
@@ -3862,8 +4498,14 @@
       <c r="I107" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J107" s="4">
+        <v>8</v>
+      </c>
+      <c r="K107" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>45002</v>
       </c>
@@ -3891,8 +4533,14 @@
       <c r="I108" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J108" s="4">
+        <v>8</v>
+      </c>
+      <c r="K108" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>45016</v>
       </c>
@@ -3920,8 +4568,14 @@
       <c r="I109" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J109" s="4">
+        <v>8</v>
+      </c>
+      <c r="K109" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44991</v>
       </c>
@@ -3949,8 +4603,14 @@
       <c r="I110" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J110" s="4">
+        <v>8</v>
+      </c>
+      <c r="K110" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44996</v>
       </c>
@@ -3978,8 +4638,14 @@
       <c r="I111" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J111" s="4">
+        <v>8</v>
+      </c>
+      <c r="K111" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44995</v>
       </c>
@@ -4007,8 +4673,14 @@
       <c r="I112" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J112" s="4">
+        <v>8</v>
+      </c>
+      <c r="K112" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44996</v>
       </c>
@@ -4036,8 +4708,14 @@
       <c r="I113" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J113" s="4">
+        <v>8</v>
+      </c>
+      <c r="K113" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44996</v>
       </c>
@@ -4065,8 +4743,14 @@
       <c r="I114" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J114" s="4">
+        <v>8</v>
+      </c>
+      <c r="K114" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44997</v>
       </c>
@@ -4094,8 +4778,14 @@
       <c r="I115" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J115" s="4">
+        <v>8</v>
+      </c>
+      <c r="K115" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44997</v>
       </c>
@@ -4123,8 +4813,14 @@
       <c r="I116" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J116" s="4">
+        <v>8</v>
+      </c>
+      <c r="K116" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44997</v>
       </c>
@@ -4152,8 +4848,14 @@
       <c r="I117" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J117" s="4">
+        <v>8</v>
+      </c>
+      <c r="K117" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>45002</v>
       </c>
@@ -4181,8 +4883,14 @@
       <c r="I118" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J118" s="4">
+        <v>4</v>
+      </c>
+      <c r="K118" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>45001</v>
       </c>
@@ -4210,8 +4918,14 @@
       <c r="I119" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J119" s="4">
+        <v>8</v>
+      </c>
+      <c r="K119" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>45002</v>
       </c>
@@ -4239,8 +4953,14 @@
       <c r="I120" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J120" s="4">
+        <v>8</v>
+      </c>
+      <c r="K120" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>45003</v>
       </c>
@@ -4268,8 +4988,14 @@
       <c r="I121" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J121" s="4">
+        <v>8</v>
+      </c>
+      <c r="K121" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>45005</v>
       </c>
@@ -4297,8 +5023,14 @@
       <c r="I122" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J122" s="4">
+        <v>8</v>
+      </c>
+      <c r="K122" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>45006</v>
       </c>
@@ -4326,8 +5058,14 @@
       <c r="I123" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J123" s="4">
+        <v>8</v>
+      </c>
+      <c r="K123" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>45005</v>
       </c>
@@ -4355,8 +5093,14 @@
       <c r="I124" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J124" s="4">
+        <v>4</v>
+      </c>
+      <c r="K124" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>45007</v>
       </c>
@@ -4384,8 +5128,14 @@
       <c r="I125" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J125" s="4">
+        <v>8</v>
+      </c>
+      <c r="K125" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>45008</v>
       </c>
@@ -4413,8 +5163,14 @@
       <c r="I126" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J126" s="4">
+        <v>8</v>
+      </c>
+      <c r="K126" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>45006</v>
       </c>
@@ -4442,8 +5198,14 @@
       <c r="I127" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J127" s="4">
+        <v>8</v>
+      </c>
+      <c r="K127" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>45012</v>
       </c>
@@ -4471,8 +5233,14 @@
       <c r="I128" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J128" s="4">
+        <v>8</v>
+      </c>
+      <c r="K128" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>45012</v>
       </c>
@@ -4500,8 +5268,14 @@
       <c r="I129" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J129" s="4">
+        <v>8</v>
+      </c>
+      <c r="K129" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>45011</v>
       </c>
@@ -4529,8 +5303,14 @@
       <c r="I130" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J130" s="4">
+        <v>8</v>
+      </c>
+      <c r="K130" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>45013</v>
       </c>
@@ -4558,8 +5338,14 @@
       <c r="I131" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J131" s="4">
+        <v>8</v>
+      </c>
+      <c r="K131" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>45013</v>
       </c>
@@ -4587,8 +5373,14 @@
       <c r="I132" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J132" s="4">
+        <v>8</v>
+      </c>
+      <c r="K132" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>45014</v>
       </c>
@@ -4616,8 +5408,14 @@
       <c r="I133" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J133" s="4">
+        <v>8</v>
+      </c>
+      <c r="K133" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44993</v>
       </c>
@@ -4645,8 +5443,14 @@
       <c r="I134" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J134" s="4">
+        <v>8</v>
+      </c>
+      <c r="K134" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44994</v>
       </c>
@@ -4674,8 +5478,14 @@
       <c r="I135" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J135" s="4">
+        <v>8</v>
+      </c>
+      <c r="K135" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44996</v>
       </c>
@@ -4703,8 +5513,14 @@
       <c r="I136" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J136" s="4">
+        <v>8</v>
+      </c>
+      <c r="K136" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>45008</v>
       </c>
@@ -4732,8 +5548,14 @@
       <c r="I137" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J137" s="4">
+        <v>8</v>
+      </c>
+      <c r="K137" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>45009</v>
       </c>
@@ -4761,8 +5583,14 @@
       <c r="I138" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J138" s="4">
+        <v>8</v>
+      </c>
+      <c r="K138" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>45009</v>
       </c>
@@ -4790,8 +5618,14 @@
       <c r="I139" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J139" s="4">
+        <v>8</v>
+      </c>
+      <c r="K139" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>45010</v>
       </c>
@@ -4819,8 +5653,14 @@
       <c r="I140" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J140" s="4">
+        <v>8</v>
+      </c>
+      <c r="K140" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>45011</v>
       </c>
@@ -4848,8 +5688,14 @@
       <c r="I141" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J141" s="4">
+        <v>8</v>
+      </c>
+      <c r="K141" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>45011</v>
       </c>
@@ -4877,8 +5723,14 @@
       <c r="I142" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J142" s="4">
+        <v>8</v>
+      </c>
+      <c r="K142" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>45011</v>
       </c>
@@ -4906,8 +5758,14 @@
       <c r="I143" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J143" s="4">
+        <v>8</v>
+      </c>
+      <c r="K143" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>45013</v>
       </c>
@@ -4935,8 +5793,14 @@
       <c r="I144" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J144" s="4">
+        <v>8</v>
+      </c>
+      <c r="K144" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>45017</v>
       </c>
@@ -4964,8 +5828,14 @@
       <c r="I145" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J145" s="4">
+        <v>8</v>
+      </c>
+      <c r="K145" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>45017</v>
       </c>
@@ -4993,8 +5863,14 @@
       <c r="I146" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J146" s="4">
+        <v>4</v>
+      </c>
+      <c r="K146" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>45017</v>
       </c>
@@ -5022,8 +5898,14 @@
       <c r="I147" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J147" s="4">
+        <v>8</v>
+      </c>
+      <c r="K147" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>45020</v>
       </c>
@@ -5051,8 +5933,14 @@
       <c r="I148" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J148" s="4">
+        <v>8</v>
+      </c>
+      <c r="K148" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>45021</v>
       </c>
@@ -5080,8 +5968,14 @@
       <c r="I149" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J149" s="4">
+        <v>8</v>
+      </c>
+      <c r="K149" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>45020</v>
       </c>
@@ -5109,8 +6003,14 @@
       <c r="I150" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J150" s="4">
+        <v>8</v>
+      </c>
+      <c r="K150" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>45023</v>
       </c>
@@ -5138,8 +6038,14 @@
       <c r="I151" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J151" s="4">
+        <v>8</v>
+      </c>
+      <c r="K151" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>45024</v>
       </c>
@@ -5167,8 +6073,14 @@
       <c r="I152" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J152" s="4">
+        <v>8</v>
+      </c>
+      <c r="K152" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>45027</v>
       </c>
@@ -5196,8 +6108,14 @@
       <c r="I153" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J153" s="4">
+        <v>8</v>
+      </c>
+      <c r="K153" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>45028</v>
       </c>
@@ -5225,8 +6143,14 @@
       <c r="I154" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J154" s="4">
+        <v>8</v>
+      </c>
+      <c r="K154" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>45028</v>
       </c>
@@ -5254,8 +6178,14 @@
       <c r="I155" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J155" s="4">
+        <v>8</v>
+      </c>
+      <c r="K155" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>45028</v>
       </c>
@@ -5283,8 +6213,14 @@
       <c r="I156" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J156" s="4">
+        <v>8</v>
+      </c>
+      <c r="K156" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>45017</v>
       </c>
@@ -5312,8 +6248,14 @@
       <c r="I157" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J157" s="4">
+        <v>4</v>
+      </c>
+      <c r="K157" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>45017</v>
       </c>
@@ -5341,8 +6283,14 @@
       <c r="I158" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J158" s="4">
+        <v>4</v>
+      </c>
+      <c r="K158" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>45020</v>
       </c>
@@ -5370,8 +6318,14 @@
       <c r="I159" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J159" s="4">
+        <v>4</v>
+      </c>
+      <c r="K159" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>45023</v>
       </c>
@@ -5399,8 +6353,14 @@
       <c r="I160" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J160" s="4">
+        <v>8</v>
+      </c>
+      <c r="K160" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>45028</v>
       </c>
@@ -5428,8 +6388,14 @@
       <c r="I161" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J161" s="4">
+        <v>4</v>
+      </c>
+      <c r="K161" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>45030</v>
       </c>
@@ -5457,8 +6423,14 @@
       <c r="I162" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J162" s="4">
+        <v>8</v>
+      </c>
+      <c r="K162" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>45024</v>
       </c>
@@ -5486,8 +6458,14 @@
       <c r="I163" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J163" s="4">
+        <v>8</v>
+      </c>
+      <c r="K163" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>45027</v>
       </c>
@@ -5515,8 +6493,14 @@
       <c r="I164" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J164" s="4">
+        <v>8</v>
+      </c>
+      <c r="K164" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>45029</v>
       </c>
@@ -5544,8 +6528,14 @@
       <c r="I165" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J165" s="4">
+        <v>8</v>
+      </c>
+      <c r="K165" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>45029</v>
       </c>
@@ -5573,8 +6563,14 @@
       <c r="I166" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J166" s="4">
+        <v>8</v>
+      </c>
+      <c r="K166" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>45031</v>
       </c>
@@ -5602,8 +6598,14 @@
       <c r="I167" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J167" s="4">
+        <v>8</v>
+      </c>
+      <c r="K167" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>45032</v>
       </c>
@@ -5631,8 +6633,14 @@
       <c r="I168" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J168" s="4">
+        <v>8</v>
+      </c>
+      <c r="K168" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>45022</v>
       </c>
@@ -5660,8 +6668,14 @@
       <c r="I169" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J169" s="4">
+        <v>8</v>
+      </c>
+      <c r="K169" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>45036</v>
       </c>
@@ -5689,8 +6703,14 @@
       <c r="I170" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J170" s="4">
+        <v>4</v>
+      </c>
+      <c r="K170" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>45032</v>
       </c>
@@ -5718,8 +6738,14 @@
       <c r="I171" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J171" s="4">
+        <v>8</v>
+      </c>
+      <c r="K171" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>45036</v>
       </c>
@@ -5747,8 +6773,14 @@
       <c r="I172" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J172" s="4">
+        <v>4</v>
+      </c>
+      <c r="K172" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>45036</v>
       </c>
@@ -5776,8 +6808,14 @@
       <c r="I173" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J173" s="4">
+        <v>8</v>
+      </c>
+      <c r="K173" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>45037</v>
       </c>
@@ -5805,8 +6843,14 @@
       <c r="I174" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J174" s="4">
+        <v>8</v>
+      </c>
+      <c r="K174" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>45039</v>
       </c>
@@ -5834,8 +6878,14 @@
       <c r="I175" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J175" s="4">
+        <v>4</v>
+      </c>
+      <c r="K175" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>45040</v>
       </c>
@@ -5863,8 +6913,14 @@
       <c r="I176" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J176" s="4">
+        <v>8</v>
+      </c>
+      <c r="K176" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>45040</v>
       </c>
@@ -5892,8 +6948,14 @@
       <c r="I177" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J177" s="4">
+        <v>8</v>
+      </c>
+      <c r="K177" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>45040</v>
       </c>
@@ -5921,8 +6983,14 @@
       <c r="I178" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J178" s="4">
+        <v>8</v>
+      </c>
+      <c r="K178" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>45044</v>
       </c>
@@ -5950,8 +7018,14 @@
       <c r="I179" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J179" s="4">
+        <v>8</v>
+      </c>
+      <c r="K179" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>45042</v>
       </c>
@@ -5979,8 +7053,14 @@
       <c r="I180" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J180" s="4">
+        <v>4</v>
+      </c>
+      <c r="K180" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>45044</v>
       </c>
@@ -6008,8 +7088,14 @@
       <c r="I181" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J181" s="4">
+        <v>8</v>
+      </c>
+      <c r="K181" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>45044</v>
       </c>
@@ -6037,8 +7123,14 @@
       <c r="I182" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J182" s="4">
+        <v>4</v>
+      </c>
+      <c r="K182" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>45041</v>
       </c>
@@ -6066,8 +7158,14 @@
       <c r="I183" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J183" s="4">
+        <v>8</v>
+      </c>
+      <c r="K183" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>45043</v>
       </c>
@@ -6095,8 +7193,14 @@
       <c r="I184" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J184" s="4">
+        <v>8</v>
+      </c>
+      <c r="K184" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>45044</v>
       </c>
@@ -6124,8 +7228,14 @@
       <c r="I185" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J185" s="4">
+        <v>8</v>
+      </c>
+      <c r="K185" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>45046</v>
       </c>
@@ -6153,8 +7263,14 @@
       <c r="I186" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J186" s="4">
+        <v>8</v>
+      </c>
+      <c r="K186" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>45046</v>
       </c>
@@ -6182,8 +7298,14 @@
       <c r="I187" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J187" s="4">
+        <v>4</v>
+      </c>
+      <c r="K187" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>45047</v>
       </c>
@@ -6211,8 +7333,14 @@
       <c r="I188" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J188" s="4">
+        <v>4</v>
+      </c>
+      <c r="K188" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>45049</v>
       </c>
@@ -6240,8 +7368,14 @@
       <c r="I189" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J189" s="4">
+        <v>8</v>
+      </c>
+      <c r="K189" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>45050</v>
       </c>
@@ -6269,8 +7403,14 @@
       <c r="I190" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J190" s="4">
+        <v>8</v>
+      </c>
+      <c r="K190" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>45057</v>
       </c>
@@ -6298,8 +7438,14 @@
       <c r="I191" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J191" s="4">
+        <v>4</v>
+      </c>
+      <c r="K191" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>45057</v>
       </c>
@@ -6327,8 +7473,14 @@
       <c r="I192" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J192" s="4">
+        <v>8</v>
+      </c>
+      <c r="K192" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>45058</v>
       </c>
@@ -6356,8 +7508,14 @@
       <c r="I193" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J193" s="4">
+        <v>8</v>
+      </c>
+      <c r="K193" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>45058</v>
       </c>
@@ -6385,8 +7543,14 @@
       <c r="I194" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J194" s="4">
+        <v>4</v>
+      </c>
+      <c r="K194" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>45047</v>
       </c>
@@ -6414,8 +7578,14 @@
       <c r="I195" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J195" s="4">
+        <v>4</v>
+      </c>
+      <c r="K195" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>45047</v>
       </c>
@@ -6443,8 +7613,14 @@
       <c r="I196" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J196" s="4">
+        <v>4</v>
+      </c>
+      <c r="K196" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>45047</v>
       </c>
@@ -6472,8 +7648,14 @@
       <c r="I197" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J197" s="4">
+        <v>4</v>
+      </c>
+      <c r="K197" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>45050</v>
       </c>
@@ -6501,8 +7683,14 @@
       <c r="I198" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J198" s="4">
+        <v>4</v>
+      </c>
+      <c r="K198" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>45058</v>
       </c>
@@ -6530,8 +7718,14 @@
       <c r="I199" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J199" s="4">
+        <v>8</v>
+      </c>
+      <c r="K199" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>45048</v>
       </c>
@@ -6559,8 +7753,14 @@
       <c r="I200" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J200" s="4">
+        <v>8</v>
+      </c>
+      <c r="K200" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>45050</v>
       </c>
@@ -6588,8 +7788,14 @@
       <c r="I201" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J201" s="4">
+        <v>8</v>
+      </c>
+      <c r="K201" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>45050</v>
       </c>
@@ -6617,8 +7823,14 @@
       <c r="I202" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J202" s="4">
+        <v>8</v>
+      </c>
+      <c r="K202" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>45052</v>
       </c>
@@ -6646,8 +7858,14 @@
       <c r="I203" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J203" s="4">
+        <v>8</v>
+      </c>
+      <c r="K203" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>45055</v>
       </c>
@@ -6675,8 +7893,14 @@
       <c r="I204" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J204" s="4">
+        <v>8</v>
+      </c>
+      <c r="K204" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>45057</v>
       </c>
@@ -6704,8 +7928,14 @@
       <c r="I205" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J205" s="4">
+        <v>8</v>
+      </c>
+      <c r="K205" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>45059</v>
       </c>
@@ -6733,8 +7963,14 @@
       <c r="I206" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J206" s="4">
+        <v>8</v>
+      </c>
+      <c r="K206" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>45065</v>
       </c>
@@ -6762,8 +7998,14 @@
       <c r="I207" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J207" s="4">
+        <v>8</v>
+      </c>
+      <c r="K207" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>45065</v>
       </c>
@@ -6791,8 +8033,14 @@
       <c r="I208" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J208" s="4">
+        <v>8</v>
+      </c>
+      <c r="K208" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>45066</v>
       </c>
@@ -6820,8 +8068,14 @@
       <c r="I209" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J209" s="4">
+        <v>4</v>
+      </c>
+      <c r="K209" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>45061</v>
       </c>
@@ -6849,8 +8103,14 @@
       <c r="I210" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J210" s="4">
+        <v>8</v>
+      </c>
+      <c r="K210" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>45058</v>
       </c>
@@ -6878,8 +8138,14 @@
       <c r="I211" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J211" s="4">
+        <v>4</v>
+      </c>
+      <c r="K211" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>45066</v>
       </c>
@@ -6907,8 +8173,14 @@
       <c r="I212" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J212" s="4">
+        <v>4</v>
+      </c>
+      <c r="K212" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>45059</v>
       </c>
@@ -6936,8 +8208,14 @@
       <c r="I213" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J213" s="4">
+        <v>8</v>
+      </c>
+      <c r="K213" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>45059</v>
       </c>
@@ -6965,8 +8243,14 @@
       <c r="I214" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J214" s="4">
+        <v>8</v>
+      </c>
+      <c r="K214" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>45059</v>
       </c>
@@ -6994,8 +8278,14 @@
       <c r="I215" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J215" s="4">
+        <v>8</v>
+      </c>
+      <c r="K215" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>45062</v>
       </c>
@@ -7023,8 +8313,14 @@
       <c r="I216" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J216" s="4">
+        <v>8</v>
+      </c>
+      <c r="K216" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>45063</v>
       </c>
@@ -7052,8 +8348,14 @@
       <c r="I217" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J217" s="4">
+        <v>8</v>
+      </c>
+      <c r="K217" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>45063</v>
       </c>
@@ -7079,6 +8381,12 @@
         <v>5</v>
       </c>
       <c r="I218" s="4">
+        <v>1</v>
+      </c>
+      <c r="J218" s="4">
+        <v>8</v>
+      </c>
+      <c r="K218" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>